<commit_message>
Feat: add worksheet tabs - Skills & Interests #2 #4 - Projects #3 - Degrees & Certifications #5 - Timeline #6 - Social Links #8
</commit_message>
<xml_diff>
--- a/data/DANLSN-Tableau-Visual-Resume-2022.xlsx
+++ b/data/DANLSN-Tableau-Visual-Resume-2022.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danlsn/Documents/Projects/tableau-visual-resume/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25C1C840-6E0E-EE4D-AFE0-26E5A8AA1487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B542156-DBF9-214B-8448-F53C1E7B70FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{E1E6793C-4CAF-EF44-B929-DCA31613A1E3}"/>
+    <workbookView xWindow="17680" yWindow="760" windowWidth="16880" windowHeight="21580" activeTab="1" xr2:uid="{E1E6793C-4CAF-EF44-B929-DCA31613A1E3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Timeline" sheetId="5" r:id="rId1"/>
+    <sheet name="Social Links" sheetId="1" r:id="rId2"/>
+    <sheet name="Projects" sheetId="2" r:id="rId3"/>
+    <sheet name="Skills and Interests" sheetId="3" r:id="rId4"/>
+    <sheet name="Degrees and Certifications" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -381,6 +385,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7C91A0-0AAB-A64E-BD10-37A1B0584756}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DD711E-0DFB-A34C-BB0C-E1DBB6957166}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -392,4 +408,40 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D60CEA0-4675-F34B-9CC6-B0D9AFCD5AAB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5DF07A-CB6E-6642-86DD-E341C32251B9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636F3881-715B-8240-AA38-38AE6D7AB29D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Feat: add items to timeline worksheet #6
</commit_message>
<xml_diff>
--- a/data/DANLSN-Tableau-Visual-Resume-2022.xlsx
+++ b/data/DANLSN-Tableau-Visual-Resume-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danlsn/Documents/Projects/tableau-visual-resume/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B542156-DBF9-214B-8448-F53C1E7B70FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0760DC-49AB-8440-A2E7-7104F6341883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17680" yWindow="760" windowWidth="16880" windowHeight="21580" activeTab="1" xr2:uid="{E1E6793C-4CAF-EF44-B929-DCA31613A1E3}"/>
+    <workbookView xWindow="17680" yWindow="760" windowWidth="16880" windowHeight="21580" xr2:uid="{E1E6793C-4CAF-EF44-B929-DCA31613A1E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="5" r:id="rId1"/>
@@ -37,6 +37,263 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="84">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Start_Date</t>
+  </si>
+  <si>
+    <t>End_Date</t>
+  </si>
+  <si>
+    <t>Organisation</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Timeframe</t>
+  </si>
+  <si>
+    <t>Past</t>
+  </si>
+  <si>
+    <t>Present</t>
+  </si>
+  <si>
+    <t>Future</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Short_Title</t>
+  </si>
+  <si>
+    <t>Bachelor of Design (Architecture)</t>
+  </si>
+  <si>
+    <t>B.Architecture</t>
+  </si>
+  <si>
+    <t>Monash University</t>
+  </si>
+  <si>
+    <t>Master of Marketing (Distinction)</t>
+  </si>
+  <si>
+    <t>M.Marketing</t>
+  </si>
+  <si>
+    <t>RMIT University</t>
+  </si>
+  <si>
+    <t>Managing Director</t>
+  </si>
+  <si>
+    <t>Prop &amp; Pose Co.</t>
+  </si>
+  <si>
+    <t>PinchPoint P/L</t>
+  </si>
+  <si>
+    <t>Volunteer</t>
+  </si>
+  <si>
+    <t>Koala Kids Foundation</t>
+  </si>
+  <si>
+    <t>Data Analytics Consultant</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
+    <t>The Data School Down Under</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>Senior Data Analyst???</t>
+  </si>
+  <si>
+    <t>Snr. Data Analyst???</t>
+  </si>
+  <si>
+    <t>Data Engineer???</t>
+  </si>
+  <si>
+    <t>Data Modeller/Architect???</t>
+  </si>
+  <si>
+    <t>Data Engineering Manager???</t>
+  </si>
+  <si>
+    <t>Data Analytics Manager???</t>
+  </si>
+  <si>
+    <t>Chief Data Officer???</t>
+  </si>
+  <si>
+    <t>CDO???</t>
+  </si>
+  <si>
+    <t>Colour</t>
+  </si>
+  <si>
+    <t>Head Barista</t>
+  </si>
+  <si>
+    <t>Melbourne Grammar School</t>
+  </si>
+  <si>
+    <t>Founder</t>
+  </si>
+  <si>
+    <t>Founding Director</t>
+  </si>
+  <si>
+    <t>Daniel Lawson Photography</t>
+  </si>
+  <si>
+    <t>SONA Representative (Monash University)</t>
+  </si>
+  <si>
+    <t>SONA Representative</t>
+  </si>
+  <si>
+    <t>Australian Institute of Architects</t>
+  </si>
+  <si>
+    <t>Victorian Chapter Councillor</t>
+  </si>
+  <si>
+    <t>Chapter Councillor</t>
+  </si>
+  <si>
+    <t>Barista/Retail Assistant</t>
+  </si>
+  <si>
+    <t>Barista</t>
+  </si>
+  <si>
+    <t>Laurent Bakery</t>
+  </si>
+  <si>
+    <t>Assistant Photographer</t>
+  </si>
+  <si>
+    <t>Infusion Pictures</t>
+  </si>
+  <si>
+    <t>BARCH</t>
+  </si>
+  <si>
+    <t>MMARK</t>
+  </si>
+  <si>
+    <t>PPCO</t>
+  </si>
+  <si>
+    <t>KKF</t>
+  </si>
+  <si>
+    <t>PPPL</t>
+  </si>
+  <si>
+    <t>TDS</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DMA</t>
+  </si>
+  <si>
+    <t>DAM</t>
+  </si>
+  <si>
+    <t>DEM</t>
+  </si>
+  <si>
+    <t>CDO</t>
+  </si>
+  <si>
+    <t>HBAR</t>
+  </si>
+  <si>
+    <t>DLP</t>
+  </si>
+  <si>
+    <t>SONA</t>
+  </si>
+  <si>
+    <t>AIAVCC</t>
+  </si>
+  <si>
+    <t>APHOTO</t>
+  </si>
+  <si>
+    <t>LAURENT</t>
+  </si>
+  <si>
+    <t>GCERT</t>
+  </si>
+  <si>
+    <t>Graduate Certificate of Marketing</t>
+  </si>
+  <si>
+    <t>G.Cert Marketing</t>
+  </si>
+  <si>
+    <t>STAMB</t>
+  </si>
+  <si>
+    <t>Student Ambassador (Architecture)</t>
+  </si>
+  <si>
+    <t>Student Ambassador</t>
+  </si>
+  <si>
+    <t>TUTOR</t>
+  </si>
+  <si>
+    <t>Volunteer Tutor (Maths &amp; English)</t>
+  </si>
+  <si>
+    <t>Volunteer Tutor</t>
+  </si>
+  <si>
+    <t>MGS &amp; ACU</t>
+  </si>
+  <si>
+    <t>RCH</t>
+  </si>
+  <si>
+    <t>Registered Volunteer</t>
+  </si>
+  <si>
+    <t>The Royal Children's Hospital</t>
+  </si>
+  <si>
+    <t>MCH</t>
+  </si>
+  <si>
+    <t>Monash Childrens' Hospital</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -70,8 +327,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -87,6 +345,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DDF7DD7-E517-9D4A-AF4A-3F1A424487BE}" name="Table1" displayName="Table1" ref="A1:J25" totalsRowShown="0">
+  <autoFilter ref="A1:J25" xr:uid="{4DDF7DD7-E517-9D4A-AF4A-3F1A424487BE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J16">
+    <sortCondition ref="B1:B16"/>
+  </sortState>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{219CE53A-CCF7-3240-8512-46BB03842808}" name="ID">
+      <calculatedColumnFormula>ROW(A2)-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{4D21B159-ABE1-284C-AFDB-FDCE9F92DAFC}" name="Start_Date"/>
+    <tableColumn id="3" xr3:uid="{9D58EAC9-1986-DD4A-A0C1-9C54806DDCCE}" name="End_Date"/>
+    <tableColumn id="4" xr3:uid="{DA6B906D-E3DB-1147-A354-D68734790014}" name="Title"/>
+    <tableColumn id="5" xr3:uid="{3DB32C99-E4EC-7E49-AF9C-107C06EA4A09}" name="Short_Title"/>
+    <tableColumn id="6" xr3:uid="{A7EFB2F5-A5E3-CD4D-80B6-E0D07A4431E2}" name="Organisation"/>
+    <tableColumn id="7" xr3:uid="{028E4467-AB32-3C49-A6B5-ED9B9DA7330B}" name="Timeframe"/>
+    <tableColumn id="8" xr3:uid="{AC3135FE-E3E3-BF48-8468-106F5753B5D0}" name="Description"/>
+    <tableColumn id="10" xr3:uid="{5D17525A-8BF4-874B-B937-AF4D42180EED}" name="Colour"/>
+    <tableColumn id="9" xr3:uid="{EB8BB85C-2D20-8B43-8A8B-59CCB6CEA859}" name="Icon"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -386,13 +668,605 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7C91A0-0AAB-A64E-BD10-37A1B0584756}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1">
+        <v>40909</v>
+      </c>
+      <c r="C2" s="1">
+        <v>42185</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42036</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43646</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42552</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42735</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42736</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43830</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42614</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44711</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43647</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44834</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44593</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45688</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44835</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44592</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45689</v>
+      </c>
+      <c r="C10" s="1">
+        <v>46053</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45689</v>
+      </c>
+      <c r="C11" s="1">
+        <v>46053</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="1">
+        <v>46054</v>
+      </c>
+      <c r="C12" s="1">
+        <v>46783</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="1">
+        <v>46784</v>
+      </c>
+      <c r="C13" s="1">
+        <v>47514</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="1">
+        <v>46784</v>
+      </c>
+      <c r="C14" s="1">
+        <v>47514</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="1">
+        <v>47515</v>
+      </c>
+      <c r="C15" s="1">
+        <v>48610</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="1">
+        <v>41426</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43465</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="1">
+        <v>40544</v>
+      </c>
+      <c r="C17" s="1">
+        <v>42035</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="1">
+        <v>41640</v>
+      </c>
+      <c r="C18" s="1">
+        <v>42004</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="1">
+        <v>41640</v>
+      </c>
+      <c r="C19" s="1">
+        <v>42004</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="1">
+        <v>40969</v>
+      </c>
+      <c r="C20" s="1">
+        <v>41364</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="1">
+        <v>40878</v>
+      </c>
+      <c r="C21" s="1">
+        <v>41759</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="1">
+        <v>41275</v>
+      </c>
+      <c r="C22" s="1">
+        <v>42004</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="1">
+        <v>40179</v>
+      </c>
+      <c r="C23" s="1">
+        <v>40908</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="1">
+        <v>43101</v>
+      </c>
+      <c r="C24" s="1">
+        <v>43830</v>
+      </c>
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="1">
+        <v>43101</v>
+      </c>
+      <c r="C25" s="1">
+        <v>43830</v>
+      </c>
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -400,7 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DD711E-0DFB-A34C-BB0C-E1DBB6957166}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Feat: update timeline worksheet
</commit_message>
<xml_diff>
--- a/data/DANLSN-Tableau-Visual-Resume-2022.xlsx
+++ b/data/DANLSN-Tableau-Visual-Resume-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danlsn/Documents/Projects/tableau-visual-resume/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0760DC-49AB-8440-A2E7-7104F6341883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB5B518-4AFE-E04B-ABFB-6D2A14E290D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17680" yWindow="760" windowWidth="16880" windowHeight="21580" xr2:uid="{E1E6793C-4CAF-EF44-B929-DCA31613A1E3}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -292,6 +292,30 @@
   </si>
   <si>
     <t>Monash Childrens' Hospital</t>
+  </si>
+  <si>
+    <t>PHOTO</t>
+  </si>
+  <si>
+    <t>Contract Photographer</t>
+  </si>
+  <si>
+    <t>Photographer</t>
+  </si>
+  <si>
+    <t>Fifty Mil Studios/KIP</t>
+  </si>
+  <si>
+    <t>WEBDEV</t>
+  </si>
+  <si>
+    <t>Web Development &amp; SEO</t>
+  </si>
+  <si>
+    <t>Web Dev.</t>
+  </si>
+  <si>
+    <t>Freelance</t>
   </si>
 </sst>
 </file>
@@ -348,10 +372,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DDF7DD7-E517-9D4A-AF4A-3F1A424487BE}" name="Table1" displayName="Table1" ref="A1:J25" totalsRowShown="0">
-  <autoFilter ref="A1:J25" xr:uid="{4DDF7DD7-E517-9D4A-AF4A-3F1A424487BE}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J16">
-    <sortCondition ref="B1:B16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DDF7DD7-E517-9D4A-AF4A-3F1A424487BE}" name="Table1" displayName="Table1" ref="A1:J27" totalsRowShown="0">
+  <autoFilter ref="A1:J27" xr:uid="{4DDF7DD7-E517-9D4A-AF4A-3F1A424487BE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J27">
+    <sortCondition ref="B1:B27"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{219CE53A-CCF7-3240-8512-46BB03842808}" name="ID">
@@ -668,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7C91A0-0AAB-A64E-BD10-37A1B0584756}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,45 +742,45 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1">
-        <v>40909</v>
+        <v>40179</v>
       </c>
       <c r="C2" s="1">
-        <v>42185</v>
+        <v>40908</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1">
-        <v>42036</v>
+        <v>44197</v>
       </c>
       <c r="C3" s="1">
-        <v>43646</v>
+        <v>44834</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -764,22 +788,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1">
-        <v>42552</v>
+        <v>43831</v>
       </c>
       <c r="C4" s="1">
-        <v>42735</v>
+        <v>44834</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
@@ -787,68 +811,68 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B5" s="1">
-        <v>42736</v>
+        <v>40544</v>
       </c>
       <c r="C5" s="1">
-        <v>43830</v>
+        <v>42035</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B6" s="1">
-        <v>42614</v>
+        <v>40878</v>
       </c>
       <c r="C6" s="1">
-        <v>44711</v>
+        <v>41759</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1">
-        <v>43647</v>
+        <v>40909</v>
       </c>
       <c r="C7" s="1">
-        <v>44834</v>
+        <v>42185</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
         <v>7</v>
@@ -856,410 +880,456 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1">
-        <v>44593</v>
+        <v>40969</v>
       </c>
       <c r="C8" s="1">
-        <v>45688</v>
+        <v>41364</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B9" s="1">
-        <v>44835</v>
+        <v>41275</v>
       </c>
       <c r="C9" s="1">
-        <v>44592</v>
+        <v>42004</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1">
-        <v>45689</v>
+        <v>41426</v>
       </c>
       <c r="C10" s="1">
-        <v>46053</v>
+        <v>43465</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1">
-        <v>45689</v>
+        <v>41640</v>
       </c>
       <c r="C11" s="1">
-        <v>46053</v>
+        <v>42004</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B12" s="1">
-        <v>46054</v>
+        <v>41640</v>
       </c>
       <c r="C12" s="1">
-        <v>46783</v>
+        <v>42004</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1">
-        <v>46784</v>
+        <v>42036</v>
       </c>
       <c r="C13" s="1">
-        <v>47514</v>
+        <v>43646</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B14" s="1">
-        <v>46784</v>
+        <v>42552</v>
       </c>
       <c r="C14" s="1">
-        <v>47514</v>
+        <v>42735</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1">
-        <v>47515</v>
+        <v>42614</v>
       </c>
       <c r="C15" s="1">
-        <v>48610</v>
+        <v>44711</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1">
-        <v>41426</v>
+        <v>42736</v>
       </c>
       <c r="C16" s="1">
-        <v>43465</v>
+        <v>43830</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="G16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B17" s="1">
-        <v>40544</v>
+        <v>43101</v>
       </c>
       <c r="C17" s="1">
-        <v>42035</v>
+        <v>43830</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B18" s="1">
-        <v>41640</v>
+        <v>43101</v>
       </c>
       <c r="C18" s="1">
-        <v>42004</v>
+        <v>43830</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1">
-        <v>41640</v>
+        <v>43647</v>
       </c>
       <c r="C19" s="1">
-        <v>42004</v>
+        <v>44834</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="G19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1">
-        <v>40969</v>
+        <v>44593</v>
       </c>
       <c r="C20" s="1">
-        <v>41364</v>
+        <v>45688</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="G20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1">
-        <v>40878</v>
+        <v>44835</v>
       </c>
       <c r="C21" s="1">
-        <v>41759</v>
+        <v>44592</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="G21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1">
-        <v>41275</v>
+        <v>45689</v>
       </c>
       <c r="C22" s="1">
-        <v>42004</v>
+        <v>46053</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B23" s="1">
-        <v>40179</v>
+        <v>45689</v>
       </c>
       <c r="C23" s="1">
-        <v>40908</v>
+        <v>46053</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="F23" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="G23" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B24" s="1">
-        <v>43101</v>
+        <v>46054</v>
       </c>
       <c r="C24" s="1">
-        <v>43830</v>
+        <v>46783</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>26</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="B25" s="1">
-        <v>43101</v>
+        <v>46784</v>
       </c>
       <c r="C25" s="1">
-        <v>43830</v>
+        <v>47514</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F25" t="s">
-        <v>83</v>
+        <v>26</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="1">
+        <v>46784</v>
+      </c>
+      <c r="C26" s="1">
+        <v>47514</v>
+      </c>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="1">
+        <v>47515</v>
+      </c>
+      <c r="C27" s="1">
+        <v>48610</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat: add degrees and certifications worksheet - closes #5
</commit_message>
<xml_diff>
--- a/data/DANLSN-Tableau-Visual-Resume-2022.xlsx
+++ b/data/DANLSN-Tableau-Visual-Resume-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danlsn/Documents/Projects/tableau-visual-resume/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB5B518-4AFE-E04B-ABFB-6D2A14E290D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2455EE-E51F-4C4E-8A8F-9B58F13AA870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17680" yWindow="760" windowWidth="16880" windowHeight="21580" xr2:uid="{E1E6793C-4CAF-EF44-B929-DCA31613A1E3}"/>
+    <workbookView xWindow="17660" yWindow="760" windowWidth="16900" windowHeight="21580" activeTab="4" xr2:uid="{E1E6793C-4CAF-EF44-B929-DCA31613A1E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="104">
   <si>
     <t>ID</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Short_Title</t>
   </si>
   <si>
-    <t>Bachelor of Design (Architecture)</t>
-  </si>
-  <si>
     <t>B.Architecture</t>
   </si>
   <si>
@@ -316,6 +313,45 @@
   </si>
   <si>
     <t>Freelance</t>
+  </si>
+  <si>
+    <t>Date_Obtained</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>ALT1</t>
+  </si>
+  <si>
+    <t>ALT2</t>
+  </si>
+  <si>
+    <t>ALT3</t>
+  </si>
+  <si>
+    <t>TABLEAU</t>
+  </si>
+  <si>
+    <t>Hide</t>
+  </si>
+  <si>
+    <t>IBM Data Analyst Professional Certificate</t>
+  </si>
+  <si>
+    <t>Bachelor of Architectural Design</t>
+  </si>
+  <si>
+    <t>Alteryx Foundation Micro-Credential</t>
+  </si>
+  <si>
+    <t>Alteryx Designer Core Certification</t>
+  </si>
+  <si>
+    <t>Alteryx Designer Advanced Certification</t>
+  </si>
+  <si>
+    <t>Tableau Certified Data Analyst</t>
   </si>
 </sst>
 </file>
@@ -358,7 +394,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -390,6 +430,23 @@
     <tableColumn id="8" xr3:uid="{AC3135FE-E3E3-BF48-8468-106F5753B5D0}" name="Description"/>
     <tableColumn id="10" xr3:uid="{5D17525A-8BF4-874B-B937-AF4D42180EED}" name="Colour"/>
     <tableColumn id="9" xr3:uid="{EB8BB85C-2D20-8B43-8A8B-59CCB6CEA859}" name="Icon"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{29AC7A6D-CCAB-F743-AA78-DADDA01DC2B5}" name="Table2" displayName="Table2" ref="A1:E9" totalsRowShown="0">
+  <autoFilter ref="A1:E9" xr:uid="{29AC7A6D-CCAB-F743-AA78-DADDA01DC2B5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E9">
+    <sortCondition ref="B1:B9"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{14A4C09D-C8FA-8E4F-9F16-04B5570D08A7}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{F0AFF1BE-FED6-FA42-B5B5-718DD21C9AA0}" name="Date_Obtained" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{1D199A04-6CE1-5942-BDC2-5E6F36FEBD17}" name="Title"/>
+    <tableColumn id="4" xr3:uid="{F01B865A-972B-A845-A449-0443B6A56129}" name="Organisation"/>
+    <tableColumn id="5" xr3:uid="{16A4D71A-FD12-D440-A172-25A7396DA76E}" name="Hide"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -694,16 +751,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7C91A0-0AAB-A64E-BD10-37A1B0584756}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="12.6640625" customWidth="1"/>
   </cols>
@@ -734,7 +792,7 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J1" t="s">
         <v>10</v>
@@ -742,7 +800,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="1">
         <v>40179</v>
@@ -751,13 +809,13 @@
         <v>40908</v>
       </c>
       <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>77</v>
-      </c>
-      <c r="F2" t="s">
-        <v>78</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -765,7 +823,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1">
         <v>44197</v>
@@ -774,13 +832,13 @@
         <v>44834</v>
       </c>
       <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
         <v>85</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>86</v>
-      </c>
-      <c r="F3" t="s">
-        <v>87</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -788,7 +846,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="1">
         <v>43831</v>
@@ -797,13 +855,13 @@
         <v>44834</v>
       </c>
       <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
         <v>89</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>90</v>
-      </c>
-      <c r="F4" t="s">
-        <v>91</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
@@ -811,7 +869,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="1">
         <v>40544</v>
@@ -820,13 +878,13 @@
         <v>42035</v>
       </c>
       <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
         <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -834,7 +892,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1">
         <v>40878</v>
@@ -843,13 +901,13 @@
         <v>41759</v>
       </c>
       <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
         <v>46</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>48</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
@@ -857,7 +915,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1">
         <v>40909</v>
@@ -866,13 +924,13 @@
         <v>42185</v>
       </c>
       <c r="D7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
       </c>
       <c r="G7" t="s">
         <v>7</v>
@@ -880,7 +938,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="1">
         <v>40969</v>
@@ -889,13 +947,13 @@
         <v>41364</v>
       </c>
       <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
         <v>49</v>
-      </c>
-      <c r="E8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" t="s">
-        <v>50</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
@@ -903,7 +961,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="1">
         <v>41275</v>
@@ -912,13 +970,13 @@
         <v>42004</v>
       </c>
       <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
         <v>73</v>
       </c>
-      <c r="E9" t="s">
-        <v>74</v>
-      </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
@@ -926,7 +984,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1">
         <v>41426</v>
@@ -935,13 +993,13 @@
         <v>43465</v>
       </c>
       <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
         <v>36</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
@@ -949,7 +1007,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1">
         <v>41640</v>
@@ -958,13 +1016,13 @@
         <v>42004</v>
       </c>
       <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>42</v>
-      </c>
-      <c r="F11" t="s">
-        <v>43</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
@@ -972,7 +1030,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="1">
         <v>41640</v>
@@ -981,13 +1039,13 @@
         <v>42004</v>
       </c>
       <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
         <v>44</v>
       </c>
-      <c r="E12" t="s">
-        <v>45</v>
-      </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
@@ -995,7 +1053,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1">
         <v>42036</v>
@@ -1004,13 +1062,13 @@
         <v>43646</v>
       </c>
       <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
         <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
       </c>
       <c r="G13" t="s">
         <v>7</v>
@@ -1018,7 +1076,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="1">
         <v>42552</v>
@@ -1027,13 +1085,13 @@
         <v>42735</v>
       </c>
       <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
         <v>70</v>
       </c>
-      <c r="E14" t="s">
-        <v>71</v>
-      </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" t="s">
         <v>7</v>
@@ -1041,7 +1099,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1">
         <v>42614</v>
@@ -1050,13 +1108,13 @@
         <v>44711</v>
       </c>
       <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
         <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" t="s">
-        <v>22</v>
       </c>
       <c r="G15" t="s">
         <v>7</v>
@@ -1064,7 +1122,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1">
         <v>42736</v>
@@ -1073,13 +1131,13 @@
         <v>43830</v>
       </c>
       <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
         <v>15</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>16</v>
-      </c>
-      <c r="F16" t="s">
-        <v>17</v>
       </c>
       <c r="G16" t="s">
         <v>7</v>
@@ -1087,7 +1145,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1">
         <v>43101</v>
@@ -1096,18 +1154,18 @@
         <v>43830</v>
       </c>
       <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
         <v>80</v>
-      </c>
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="1">
         <v>43101</v>
@@ -1116,18 +1174,18 @@
         <v>43830</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1">
         <v>43647</v>
@@ -1136,13 +1194,13 @@
         <v>44834</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G19" t="s">
         <v>7</v>
@@ -1150,7 +1208,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1">
         <v>44593</v>
@@ -1159,13 +1217,13 @@
         <v>45688</v>
       </c>
       <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
         <v>23</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>24</v>
-      </c>
-      <c r="F20" t="s">
-        <v>25</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
@@ -1173,7 +1231,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1">
         <v>44835</v>
@@ -1182,13 +1240,13 @@
         <v>44592</v>
       </c>
       <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
         <v>23</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>24</v>
-      </c>
-      <c r="F21" t="s">
-        <v>25</v>
       </c>
       <c r="G21" t="s">
         <v>7</v>
@@ -1196,7 +1254,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1">
         <v>45689</v>
@@ -1205,13 +1263,13 @@
         <v>46053</v>
       </c>
       <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
         <v>27</v>
       </c>
-      <c r="E22" t="s">
-        <v>28</v>
-      </c>
       <c r="F22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G22" t="s">
         <v>8</v>
@@ -1219,7 +1277,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="1">
         <v>45689</v>
@@ -1228,13 +1286,13 @@
         <v>46053</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G23" t="s">
         <v>8</v>
@@ -1242,7 +1300,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="1">
         <v>46054</v>
@@ -1251,13 +1309,13 @@
         <v>46783</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
@@ -1265,7 +1323,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1">
         <v>46784</v>
@@ -1274,13 +1332,13 @@
         <v>47514</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G25" t="s">
         <v>8</v>
@@ -1288,7 +1346,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="1">
         <v>46784</v>
@@ -1297,13 +1355,13 @@
         <v>47514</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G26" t="s">
         <v>8</v>
@@ -1311,7 +1369,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="1">
         <v>47515</v>
@@ -1320,13 +1378,13 @@
         <v>48610</v>
       </c>
       <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" t="s">
         <v>33</v>
       </c>
-      <c r="E27" t="s">
-        <v>34</v>
-      </c>
       <c r="F27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G27" t="s">
         <v>8</v>
@@ -1380,12 +1438,132 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636F3881-715B-8240-AA38-38AE6D7AB29D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1">
+        <v>42125</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42705</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43800</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44542</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44842</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44844</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feat: convert svg icons to png
</commit_message>
<xml_diff>
--- a/data/DANLSN-Tableau-Visual-Resume-2022.xlsx
+++ b/data/DANLSN-Tableau-Visual-Resume-2022.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danlsn/Documents/Projects/tableau-visual-resume/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2455EE-E51F-4C4E-8A8F-9B58F13AA870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2335F5B0-162D-1144-BFA4-22F093F3C739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17660" yWindow="760" windowWidth="16900" windowHeight="21580" activeTab="4" xr2:uid="{E1E6793C-4CAF-EF44-B929-DCA31613A1E3}"/>
+    <workbookView xWindow="-1460" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{E1E6793C-4CAF-EF44-B929-DCA31613A1E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="5" r:id="rId1"/>
-    <sheet name="Social Links" sheetId="1" r:id="rId2"/>
-    <sheet name="Projects" sheetId="2" r:id="rId3"/>
-    <sheet name="Skills and Interests" sheetId="3" r:id="rId4"/>
-    <sheet name="Degrees and Certifications" sheetId="4" r:id="rId5"/>
+    <sheet name="Degrees and Certifications" sheetId="4" r:id="rId2"/>
+    <sheet name="Social Links" sheetId="1" r:id="rId3"/>
+    <sheet name="Projects" sheetId="2" r:id="rId4"/>
+    <sheet name="Skills and Interests" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="130">
   <si>
     <t>ID</t>
   </si>
@@ -352,16 +352,102 @@
   </si>
   <si>
     <t>Tableau Certified Data Analyst</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Handle</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>https://danlsn.com.au</t>
+  </si>
+  <si>
+    <t>https://www.thedataschool.com.au/the-team/daniel-lawson</t>
+  </si>
+  <si>
+    <t>https://github.com/danlsn</t>
+  </si>
+  <si>
+    <t>https://twitter.com/_danlsn</t>
+  </si>
+  <si>
+    <t>https://linkedin.com/in/danlsn</t>
+  </si>
+  <si>
+    <t>https://instagram.com/_danlsn</t>
+  </si>
+  <si>
+    <t>@danlsn</t>
+  </si>
+  <si>
+    <t>@_danlsn</t>
+  </si>
+  <si>
+    <t>Reddit</t>
+  </si>
+  <si>
+    <t>https://reddit.com/u/danlsn</t>
+  </si>
+  <si>
+    <t>WEB</t>
+  </si>
+  <si>
+    <t>DSAU</t>
+  </si>
+  <si>
+    <t>GITHUB</t>
+  </si>
+  <si>
+    <t>TWITTER</t>
+  </si>
+  <si>
+    <t>LINKEDIN</t>
+  </si>
+  <si>
+    <t>INSTA</t>
+  </si>
+  <si>
+    <t>REDDIT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -384,14 +470,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -447,6 +537,20 @@
     <tableColumn id="3" xr3:uid="{1D199A04-6CE1-5942-BDC2-5E6F36FEBD17}" name="Title"/>
     <tableColumn id="4" xr3:uid="{F01B865A-972B-A845-A449-0443B6A56129}" name="Organisation"/>
     <tableColumn id="5" xr3:uid="{16A4D71A-FD12-D440-A172-25A7396DA76E}" name="Hide"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{33B70E93-39AC-284D-A64E-4B2660F423E9}" name="Table3" displayName="Table3" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8" xr:uid="{33B70E93-39AC-284D-A64E-4B2660F423E9}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{DAB00A8A-C286-8442-909D-EDC8696AF7E1}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{19C1BEFC-C78A-444D-9652-0CDA68949E72}" name="Platform"/>
+    <tableColumn id="3" xr3:uid="{7F0A8F9D-90D5-8242-868C-4C7CD5D1246D}" name="URL" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{E54409A5-F44F-C348-8FC3-9562AA3A4299}" name="Handle"/>
+    <tableColumn id="5" xr3:uid="{A8B18CDB-45B2-4F46-B6F2-8F732E4FEB5F}" name="Icon"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1399,48 +1503,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DD711E-0DFB-A34C-BB0C-E1DBB6957166}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D60CEA0-4675-F34B-9CC6-B0D9AFCD5AAB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5DF07A-CB6E-6642-86DD-E341C32251B9}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636F3881-715B-8240-AA38-38AE6D7AB29D}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1566,4 +1632,167 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DD711E-0DFB-A34C-BB0C-E1DBB6957166}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{872680AD-F07E-2041-B49C-80BD1E355D40}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{687585A4-99AF-1E4A-A482-6B41D1E16B8D}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{B7CB83F9-4DD1-CE42-9D45-F6BB51E564AA}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{95111099-FD12-C645-9D01-63BD24F97842}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{8B2584F9-002E-6349-ABA2-A091EACBEF9A}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{DF2E71F8-2ADE-3745-A7C5-BE642537F95D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId7"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D60CEA0-4675-F34B-9CC6-B0D9AFCD5AAB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5DF07A-CB6E-6642-86DD-E341C32251B9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Feat: update spreadsheet data
</commit_message>
<xml_diff>
--- a/data/DANLSN-Tableau-Visual-Resume-2022.xlsx
+++ b/data/DANLSN-Tableau-Visual-Resume-2022.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danlsn/Documents/Projects/tableau-visual-resume/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielLawson\IdeaProjects\tableau-visual-resume\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F2A25C-8B0E-4849-859B-DA334B55AC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2A8918-A0D1-4E5F-8CE4-9C5D98FE8816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1460" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{E1E6793C-4CAF-EF44-B929-DCA31613A1E3}"/>
+    <workbookView xWindow="2220" yWindow="2115" windowWidth="21600" windowHeight="11295" xr2:uid="{E1E6793C-4CAF-EF44-B929-DCA31613A1E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="5" r:id="rId1"/>
     <sheet name="Degrees and Certifications" sheetId="4" r:id="rId2"/>
     <sheet name="Social Links" sheetId="1" r:id="rId3"/>
     <sheet name="Projects" sheetId="2" r:id="rId4"/>
-    <sheet name="Skills and Interests" sheetId="3" r:id="rId5"/>
+    <sheet name="Skills-to-Projects" sheetId="6" r:id="rId5"/>
+    <sheet name="Skills and Interests" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="306">
   <si>
     <t>ID</t>
   </si>
@@ -108,9 +109,6 @@
     <t>Koala Kids Foundation</t>
   </si>
   <si>
-    <t>Data Analytics Consultant</t>
-  </si>
-  <si>
     <t>Data Analyst</t>
   </si>
   <si>
@@ -339,9 +337,6 @@
     <t>IBM Data Analyst Professional Certificate</t>
   </si>
   <si>
-    <t>Bachelor of Architectural Design</t>
-  </si>
-  <si>
     <t>Alteryx Foundation Micro-Credential</t>
   </si>
   <si>
@@ -919,6 +914,51 @@
   </si>
   <si>
     <t>R Language</t>
+  </si>
+  <si>
+    <t>TDSF</t>
+  </si>
+  <si>
+    <t>Data Analytics Consultant — Training</t>
+  </si>
+  <si>
+    <t>Data Analytics Consultant — Placements</t>
+  </si>
+  <si>
+    <t>Skill_ID</t>
+  </si>
+  <si>
+    <t>Project_ID</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>https://github.com/danlsn/tableau-visual-resume/raw/main/media/icons/heart.png</t>
+  </si>
+  <si>
+    <t>https://github.com/danlsn/tableau-visual-resume/raw/main/media/icons/recycle.png</t>
+  </si>
+  <si>
+    <t>https://github.com/danlsn/tableau-visual-resume/raw/main/media/icons/crown.png</t>
+  </si>
+  <si>
+    <t>https://github.com/danlsn/tableau-visual-resume/raw/main/media/icons/brain.png</t>
+  </si>
+  <si>
+    <t>https://github.com/danlsn/tableau-visual-resume/raw/main/media/icons/synthesizer.png</t>
+  </si>
+  <si>
+    <t>Top-Level Skill</t>
+  </si>
+  <si>
+    <t>Photography &amp; Videography</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>Bachelor of Architecture</t>
   </si>
 </sst>
 </file>
@@ -942,15 +982,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -958,24 +1004,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1022,7 +1098,7 @@
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{14A4C09D-C8FA-8E4F-9F16-04B5570D08A7}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{F0AFF1BE-FED6-FA42-B5B5-718DD21C9AA0}" name="Date_Obtained" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{F0AFF1BE-FED6-FA42-B5B5-718DD21C9AA0}" name="Date_Obtained" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{1D199A04-6CE1-5942-BDC2-5E6F36FEBD17}" name="Title"/>
     <tableColumn id="4" xr3:uid="{F01B865A-972B-A845-A449-0443B6A56129}" name="Organisation"/>
     <tableColumn id="5" xr3:uid="{16A4D71A-FD12-D440-A172-25A7396DA76E}" name="Hide"/>
@@ -1046,13 +1122,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D5531047-723A-E944-B794-8E7F8322F364}" name="Table4" displayName="Table4" ref="A1:E23" totalsRowShown="0">
-  <autoFilter ref="A1:E23" xr:uid="{D5531047-723A-E944-B794-8E7F8322F364}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D5531047-723A-E944-B794-8E7F8322F364}" name="Table4" displayName="Table4" ref="A1:H23" totalsRowShown="0">
+  <autoFilter ref="A1:H23" xr:uid="{D5531047-723A-E944-B794-8E7F8322F364}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{D829FA3D-206C-6B42-8EA8-0BEF1CF8FF40}" name="ID"/>
+    <tableColumn id="6" xr3:uid="{E05D4F10-5705-4C98-B0A0-788168521B99}" name="Order"/>
+    <tableColumn id="7" xr3:uid="{62D560B5-B109-463D-8A47-27C3F2B584E9}" name="Hide"/>
     <tableColumn id="2" xr3:uid="{6C4E7434-15B8-E64A-8BE3-C9BE597FC5C6}" name="Title"/>
     <tableColumn id="3" xr3:uid="{352104A3-A730-DD4D-9F4D-95F8FDBC357A}" name="Client"/>
     <tableColumn id="4" xr3:uid="{2EF8B096-72AE-C245-A4B8-6E99C12A060A}" name="Description"/>
+    <tableColumn id="8" xr3:uid="{24D8EE8F-5FDB-4F34-8320-9F0758FF03A6}" name="Icon"/>
     <tableColumn id="5" xr3:uid="{001B6D29-EEBD-A54D-891F-CD2E98EDA111}" name="URL"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1060,12 +1139,24 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BEF4B8A2-1252-1449-AF5F-F3EC0BA37BA5}" name="Table5" displayName="Table5" ref="A1:F42" totalsRowShown="0">
-  <autoFilter ref="A1:F42" xr:uid="{BEF4B8A2-1252-1449-AF5F-F3EC0BA37BA5}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D75B64CD-95E9-4F6D-A0D3-EACF0897E535}" name="Table6" displayName="Table6" ref="A1:B63" totalsRowShown="0">
+  <autoFilter ref="A1:B63" xr:uid="{D75B64CD-95E9-4F6D-A0D3-EACF0897E535}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{9F199608-C5F4-4C69-895F-CFCC51810421}" name="Project_ID" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{E44F2412-64FC-4B47-B7A1-4A760994E339}" name="Skill_ID"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BEF4B8A2-1252-1449-AF5F-F3EC0BA37BA5}" name="Table5" displayName="Table5" ref="A1:G43" totalsRowShown="0">
+  <autoFilter ref="A1:G43" xr:uid="{BEF4B8A2-1252-1449-AF5F-F3EC0BA37BA5}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{8144B610-625C-304B-BB02-ED98C5A14C99}" name="ID"/>
     <tableColumn id="2" xr3:uid="{3312C1D9-B2E9-3448-AE31-9F1160CAA3E1}" name="Skill"/>
     <tableColumn id="3" xr3:uid="{CFCD893B-FF40-6847-9082-B1DB0D6B95E5}" name="Type"/>
+    <tableColumn id="7" xr3:uid="{376B1D72-C741-470C-9C0E-078DD8355563}" name="Top-Level Skill"/>
     <tableColumn id="4" xr3:uid="{F28D44CF-8C8C-4048-8688-758438341697}" name="Parent"/>
     <tableColumn id="5" xr3:uid="{31E796B6-489E-674F-ABE4-97B02BF85DFA}" name="Technical"/>
     <tableColumn id="6" xr3:uid="{DEDAC0C6-6499-4744-B9C2-15306BE4B24F}" name="Familiar-Comfortable-Confident"/>
@@ -1075,7 +1166,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1363,7 +1454,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1373,22 +1464,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7C91A0-0AAB-A64E-BD10-37A1B0584756}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1414,15 +1505,15 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="1">
         <v>40179</v>
@@ -1431,21 +1522,21 @@
         <v>40908</v>
       </c>
       <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" t="s">
         <v>75</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>77</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1">
         <v>44197</v>
@@ -1454,21 +1545,21 @@
         <v>44834</v>
       </c>
       <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>84</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>85</v>
-      </c>
-      <c r="F3" t="s">
-        <v>86</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1">
         <v>43831</v>
@@ -1477,21 +1568,21 @@
         <v>44834</v>
       </c>
       <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
         <v>88</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>89</v>
-      </c>
-      <c r="F4" t="s">
-        <v>90</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1">
         <v>40544</v>
@@ -1500,21 +1591,21 @@
         <v>42035</v>
       </c>
       <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
         <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1">
         <v>40878</v>
@@ -1523,21 +1614,21 @@
         <v>41759</v>
       </c>
       <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
         <v>45</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>46</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1">
         <v>40909</v>
@@ -1546,7 +1637,7 @@
         <v>42185</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>305</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -1558,9 +1649,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1">
         <v>40969</v>
@@ -1569,21 +1660,21 @@
         <v>41364</v>
       </c>
       <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
         <v>48</v>
-      </c>
-      <c r="E8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1">
         <v>41275</v>
@@ -1592,10 +1683,10 @@
         <v>42004</v>
       </c>
       <c r="D9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" t="s">
         <v>72</v>
-      </c>
-      <c r="E9" t="s">
-        <v>73</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
@@ -1604,9 +1695,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1">
         <v>41426</v>
@@ -1615,21 +1706,21 @@
         <v>43465</v>
       </c>
       <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
         <v>35</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="1">
         <v>41640</v>
@@ -1638,21 +1729,21 @@
         <v>42004</v>
       </c>
       <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>41</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="1">
         <v>41640</v>
@@ -1661,21 +1752,21 @@
         <v>42004</v>
       </c>
       <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
         <v>43</v>
       </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1">
         <v>42036</v>
@@ -1696,9 +1787,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="1">
         <v>42552</v>
@@ -1707,21 +1798,21 @@
         <v>42735</v>
       </c>
       <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s">
         <v>69</v>
-      </c>
-      <c r="E14" t="s">
-        <v>70</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="1">
         <v>42614</v>
@@ -1742,9 +1833,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1">
         <v>42736</v>
@@ -1765,9 +1856,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" s="1">
         <v>43101</v>
@@ -1776,18 +1867,21 @@
         <v>43830</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
         <v>20</v>
       </c>
       <c r="F17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>81</v>
       </c>
       <c r="B18" s="1">
         <v>43101</v>
@@ -1796,18 +1890,21 @@
         <v>43830</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
         <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1">
         <v>43647</v>
@@ -1828,55 +1925,55 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>291</v>
       </c>
       <c r="B20" s="1">
-        <v>44593</v>
+        <v>44958</v>
       </c>
       <c r="C20" s="1">
         <v>45688</v>
       </c>
       <c r="D20" t="s">
+        <v>293</v>
+      </c>
+      <c r="E20" t="s">
         <v>22</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>23</v>
       </c>
-      <c r="F20" t="s">
-        <v>24</v>
-      </c>
       <c r="G20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1">
         <v>44835</v>
       </c>
       <c r="C21" s="1">
-        <v>44592</v>
+        <v>44957</v>
       </c>
       <c r="D21" t="s">
+        <v>292</v>
+      </c>
+      <c r="E21" t="s">
         <v>22</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>23</v>
-      </c>
-      <c r="F21" t="s">
-        <v>24</v>
       </c>
       <c r="G21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1">
         <v>45689</v>
@@ -1885,21 +1982,21 @@
         <v>46053</v>
       </c>
       <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" t="s">
         <v>26</v>
       </c>
-      <c r="E22" t="s">
-        <v>27</v>
-      </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1">
         <v>45689</v>
@@ -1908,21 +2005,21 @@
         <v>46053</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1">
         <v>46054</v>
@@ -1931,21 +2028,21 @@
         <v>46783</v>
       </c>
       <c r="D24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1">
         <v>46784</v>
@@ -1954,21 +2051,21 @@
         <v>47514</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1">
         <v>46784</v>
@@ -1977,21 +2074,21 @@
         <v>47514</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" s="1">
         <v>47515</v>
@@ -2000,13 +2097,13 @@
         <v>48610</v>
       </c>
       <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" t="s">
         <v>32</v>
       </c>
-      <c r="E27" t="s">
-        <v>33</v>
-      </c>
       <c r="F27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G27" t="s">
         <v>8</v>
@@ -2025,23 +2122,23 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
     <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="7.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -2050,40 +2147,40 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1">
         <v>42125</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>305</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1">
         <v>42705</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1">
         <v>43800</v>
@@ -2095,74 +2192,74 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="1">
         <v>44542</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="1">
         <v>44842</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="1">
         <v>44844</v>
       </c>
       <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" t="s">
         <v>101</v>
       </c>
-      <c r="D7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" t="s">
-        <v>201</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" t="s">
-        <v>103</v>
-      </c>
       <c r="D9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2184,152 +2281,152 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="53.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
         <v>104</v>
-      </c>
-      <c r="C1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" t="s">
-        <v>106</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>123</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>124</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>125</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
         <v>119</v>
       </c>
-      <c r="E4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2351,937 +2448,1595 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D60CEA0-4675-F34B-9CC6-B0D9AFCD5AAB}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="83.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="83.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" t="s">
         <v>155</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="G3" t="s">
+        <v>298</v>
+      </c>
+      <c r="H3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>176</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>136</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" t="s">
+        <v>299</v>
+      </c>
+      <c r="H4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="H5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>299</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" t="s">
+        <v>154</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G9" t="s">
+        <v>301</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" t="s">
+        <v>154</v>
+      </c>
+      <c r="H10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" t="s">
         <v>156</v>
       </c>
-      <c r="E2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G12" t="s">
+        <v>298</v>
+      </c>
+      <c r="H12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>184</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" t="s">
         <v>156</v>
       </c>
-      <c r="E4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="H13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" t="s">
         <v>156</v>
       </c>
-      <c r="E5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="G14" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" t="s">
+        <v>154</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" t="s">
+        <v>154</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" t="s">
         <v>156</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>197</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="G17" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" t="s">
         <v>156</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" t="s">
         <v>156</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>183</v>
-      </c>
-      <c r="B10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" t="s">
         <v>156</v>
       </c>
-      <c r="E10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>184</v>
-      </c>
-      <c r="B11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>192</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21" t="s">
         <v>156</v>
       </c>
-      <c r="E11" t="s">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>185</v>
-      </c>
-      <c r="B12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>186</v>
-      </c>
-      <c r="B13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="E22" t="s">
+        <v>156</v>
+      </c>
+      <c r="H22" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>187</v>
-      </c>
-      <c r="B14" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14" t="s">
-        <v>158</v>
-      </c>
-      <c r="E14" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" t="s">
+        <v>154</v>
+      </c>
+      <c r="H23" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>188</v>
-      </c>
-      <c r="B15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C15" t="s">
-        <v>156</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>189</v>
-      </c>
-      <c r="B16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C16" t="s">
-        <v>156</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>190</v>
-      </c>
-      <c r="B17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>191</v>
-      </c>
-      <c r="B18" t="s">
-        <v>151</v>
-      </c>
-      <c r="C18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>192</v>
-      </c>
-      <c r="B19" t="s">
-        <v>152</v>
-      </c>
-      <c r="C19" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>193</v>
-      </c>
-      <c r="B20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B21" t="s">
-        <v>154</v>
-      </c>
-      <c r="C21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" t="s">
-        <v>166</v>
-      </c>
-      <c r="C22" t="s">
-        <v>158</v>
-      </c>
-      <c r="E22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>195</v>
-      </c>
-      <c r="B23" t="s">
-        <v>168</v>
-      </c>
-      <c r="C23" t="s">
-        <v>156</v>
-      </c>
-      <c r="E23" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" xr:uid="{A2EB1769-670D-D048-B933-C02CC07BA0E6}"/>
-    <hyperlink ref="E6" r:id="rId2" xr:uid="{1E7DBEC6-398B-6C44-8E40-18F47FAC9559}"/>
-    <hyperlink ref="E8" r:id="rId3" xr:uid="{C5FF54AB-90FC-1341-A23A-DEBC3F1E44B6}"/>
-    <hyperlink ref="E7" r:id="rId4" xr:uid="{C996C626-DBA5-E145-9AF7-C6B327D9487D}"/>
-    <hyperlink ref="E15" r:id="rId5" xr:uid="{D3BDDBF4-4DA5-6845-A452-F7BAA5414751}"/>
-    <hyperlink ref="E16" r:id="rId6" xr:uid="{0D320689-50C0-CB44-B7BC-7F15ED2B2F56}"/>
+    <hyperlink ref="H9" r:id="rId1" xr:uid="{A2EB1769-670D-D048-B933-C02CC07BA0E6}"/>
+    <hyperlink ref="H6" r:id="rId2" xr:uid="{1E7DBEC6-398B-6C44-8E40-18F47FAC9559}"/>
+    <hyperlink ref="H8" r:id="rId3" xr:uid="{C5FF54AB-90FC-1341-A23A-DEBC3F1E44B6}"/>
+    <hyperlink ref="H7" r:id="rId4" xr:uid="{C996C626-DBA5-E145-9AF7-C6B327D9487D}"/>
+    <hyperlink ref="H15" r:id="rId5" xr:uid="{D3BDDBF4-4DA5-6845-A452-F7BAA5414751}"/>
+    <hyperlink ref="H16" r:id="rId6" xr:uid="{0D320689-50C0-CB44-B7BC-7F15ED2B2F56}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{4703C837-CC40-4EBF-AB41-F866044EE5C2}"/>
+    <hyperlink ref="G6" r:id="rId8" xr:uid="{3EDAAD96-3653-4ADF-AA17-DAE2FCCD3B78}"/>
+    <hyperlink ref="G8" r:id="rId9" xr:uid="{9FCE2417-6186-402A-9155-9E0B70F199E9}"/>
+    <hyperlink ref="G14" r:id="rId10" xr:uid="{17AF2D8A-4ADF-4369-8C7D-4450B57013F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5DF07A-CB6E-6642-86DD-E341C32251B9}">
-  <dimension ref="A1:F42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59DD3FA5-56CC-40F9-B1FB-2128066476D7}">
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5DF07A-CB6E-6642-86DD-E341C32251B9}">
+  <dimension ref="A1:G43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.875" customWidth="1"/>
+    <col min="5" max="5" width="8.875" customWidth="1"/>
+    <col min="6" max="6" width="11.125" customWidth="1"/>
+    <col min="7" max="7" width="29.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" t="s">
         <v>203</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>245</v>
       </c>
-      <c r="D1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E3" t="s">
         <v>242</v>
       </c>
-      <c r="F1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" t="s">
+        <v>251</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>283</v>
+      </c>
+      <c r="B6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" t="s">
+        <v>246</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>281</v>
+      </c>
+      <c r="B8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C8" t="s">
+        <v>248</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C9" t="s">
+        <v>247</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C10" t="s">
+        <v>247</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>254</v>
+      </c>
+      <c r="B11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" t="s">
+        <v>247</v>
+      </c>
+      <c r="E11" t="s">
+        <v>211</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" t="s">
+        <v>246</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13" t="s">
+        <v>199</v>
+      </c>
+      <c r="C13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" t="s">
         <v>244</v>
       </c>
-      <c r="B2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15" t="s">
+        <v>214</v>
+      </c>
+      <c r="C15" t="s">
+        <v>251</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" t="s">
+        <v>238</v>
+      </c>
+      <c r="C16" t="s">
+        <v>249</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>258</v>
+      </c>
+      <c r="B17" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" t="s">
+        <v>249</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>259</v>
+      </c>
+      <c r="B18" t="s">
+        <v>217</v>
+      </c>
+      <c r="C18" t="s">
+        <v>249</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B19" t="s">
+        <v>218</v>
+      </c>
+      <c r="C19" t="s">
+        <v>250</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>261</v>
+      </c>
+      <c r="B20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C20" t="s">
+        <v>246</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>262</v>
+      </c>
+      <c r="B21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" t="s">
+        <v>245</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>263</v>
+      </c>
+      <c r="B22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C22" t="s">
+        <v>245</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>264</v>
+      </c>
+      <c r="B23" t="s">
+        <v>222</v>
+      </c>
+      <c r="C23" t="s">
+        <v>248</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>265</v>
+      </c>
+      <c r="B24" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" t="s">
+        <v>251</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>266</v>
+      </c>
+      <c r="B25" t="s">
+        <v>224</v>
+      </c>
+      <c r="C25" t="s">
+        <v>251</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>267</v>
+      </c>
+      <c r="B26" t="s">
+        <v>225</v>
+      </c>
+      <c r="C26" t="s">
         <v>247</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>268</v>
+      </c>
+      <c r="B27" t="s">
+        <v>226</v>
+      </c>
+      <c r="C27" t="s">
+        <v>249</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>269</v>
+      </c>
+      <c r="B28" t="s">
+        <v>227</v>
+      </c>
+      <c r="C28" t="s">
+        <v>249</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>270</v>
+      </c>
+      <c r="B29" t="s">
+        <v>228</v>
+      </c>
+      <c r="C29" t="s">
+        <v>252</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>271</v>
+      </c>
+      <c r="B30" t="s">
+        <v>229</v>
+      </c>
+      <c r="C30" t="s">
+        <v>253</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>272</v>
+      </c>
+      <c r="B31" t="s">
+        <v>230</v>
+      </c>
+      <c r="C31" t="s">
+        <v>250</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>273</v>
+      </c>
+      <c r="B32" t="s">
+        <v>231</v>
+      </c>
+      <c r="C32" t="s">
+        <v>253</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>274</v>
+      </c>
+      <c r="B33" t="s">
+        <v>232</v>
+      </c>
+      <c r="C33" t="s">
+        <v>253</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>275</v>
+      </c>
+      <c r="B34" t="s">
+        <v>233</v>
+      </c>
+      <c r="C34" t="s">
+        <v>253</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>276</v>
+      </c>
+      <c r="B35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C35" t="s">
+        <v>253</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>277</v>
+      </c>
+      <c r="B36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C36" t="s">
+        <v>253</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" t="s">
+        <v>236</v>
+      </c>
+      <c r="C37" t="s">
+        <v>251</v>
+      </c>
+      <c r="G37">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>278</v>
+      </c>
+      <c r="B38" t="s">
+        <v>237</v>
+      </c>
+      <c r="C38" t="s">
+        <v>252</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>279</v>
+      </c>
+      <c r="B39" t="s">
+        <v>239</v>
+      </c>
+      <c r="C39" t="s">
+        <v>247</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>287</v>
+      </c>
+      <c r="C40" t="s">
+        <v>248</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>304</v>
+      </c>
+      <c r="B41" t="s">
         <v>288</v>
       </c>
-      <c r="B3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" t="s">
-        <v>247</v>
-      </c>
-      <c r="D3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>287</v>
-      </c>
-      <c r="B4" t="s">
-        <v>207</v>
-      </c>
-      <c r="C4" t="s">
-        <v>250</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>286</v>
-      </c>
-      <c r="B5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C5" t="s">
-        <v>253</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>285</v>
-      </c>
-      <c r="B6" t="s">
-        <v>209</v>
-      </c>
-      <c r="C6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D6" t="s">
-        <v>244</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>284</v>
-      </c>
-      <c r="B7" t="s">
-        <v>210</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C41" t="s">
         <v>248</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>283</v>
-      </c>
-      <c r="B8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" t="s">
-        <v>250</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>282</v>
-      </c>
-      <c r="B9" t="s">
-        <v>212</v>
-      </c>
-      <c r="C9" t="s">
-        <v>249</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>213</v>
-      </c>
-      <c r="B10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C10" t="s">
-        <v>249</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>256</v>
-      </c>
-      <c r="B11" t="s">
-        <v>214</v>
-      </c>
-      <c r="C11" t="s">
-        <v>249</v>
-      </c>
-      <c r="D11" t="s">
-        <v>213</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C12" t="s">
-        <v>248</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>257</v>
-      </c>
-      <c r="B13" t="s">
-        <v>201</v>
-      </c>
-      <c r="C13" t="s">
-        <v>250</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>258</v>
-      </c>
-      <c r="B14" t="s">
-        <v>215</v>
-      </c>
-      <c r="C14" t="s">
-        <v>246</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>259</v>
-      </c>
-      <c r="B15" t="s">
-        <v>216</v>
-      </c>
-      <c r="C15" t="s">
-        <v>253</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>217</v>
-      </c>
-      <c r="B16" t="s">
-        <v>240</v>
-      </c>
-      <c r="C16" t="s">
-        <v>251</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>260</v>
-      </c>
-      <c r="B17" t="s">
-        <v>218</v>
-      </c>
-      <c r="C17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>261</v>
-      </c>
-      <c r="B18" t="s">
-        <v>219</v>
-      </c>
-      <c r="C18" t="s">
-        <v>251</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>262</v>
-      </c>
-      <c r="B19" t="s">
-        <v>220</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>303</v>
+      </c>
+      <c r="C42" t="s">
         <v>252</v>
       </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>263</v>
-      </c>
-      <c r="B20" t="s">
-        <v>221</v>
-      </c>
-      <c r="C20" t="s">
-        <v>248</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>264</v>
-      </c>
-      <c r="B21" t="s">
-        <v>222</v>
-      </c>
-      <c r="C21" t="s">
-        <v>247</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>265</v>
-      </c>
-      <c r="B22" t="s">
-        <v>223</v>
-      </c>
-      <c r="C22" t="s">
-        <v>247</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>266</v>
-      </c>
-      <c r="B23" t="s">
-        <v>224</v>
-      </c>
-      <c r="C23" t="s">
-        <v>250</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>267</v>
-      </c>
-      <c r="B24" t="s">
-        <v>225</v>
-      </c>
-      <c r="C24" t="s">
-        <v>253</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>268</v>
-      </c>
-      <c r="B25" t="s">
-        <v>226</v>
-      </c>
-      <c r="C25" t="s">
-        <v>253</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>269</v>
-      </c>
-      <c r="B26" t="s">
-        <v>227</v>
-      </c>
-      <c r="C26" t="s">
-        <v>249</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>270</v>
-      </c>
-      <c r="B27" t="s">
-        <v>228</v>
-      </c>
-      <c r="C27" t="s">
-        <v>251</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>271</v>
-      </c>
-      <c r="B28" t="s">
-        <v>229</v>
-      </c>
-      <c r="C28" t="s">
-        <v>251</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>272</v>
-      </c>
-      <c r="B29" t="s">
-        <v>230</v>
-      </c>
-      <c r="C29" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>273</v>
-      </c>
-      <c r="B30" t="s">
-        <v>231</v>
-      </c>
-      <c r="C30" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>274</v>
-      </c>
-      <c r="B31" t="s">
-        <v>232</v>
-      </c>
-      <c r="C31" t="s">
-        <v>252</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>275</v>
-      </c>
-      <c r="B32" t="s">
-        <v>233</v>
-      </c>
-      <c r="C32" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>276</v>
-      </c>
-      <c r="B33" t="s">
-        <v>234</v>
-      </c>
-      <c r="C33" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>277</v>
-      </c>
-      <c r="B34" t="s">
-        <v>235</v>
-      </c>
-      <c r="C34" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>278</v>
-      </c>
-      <c r="B35" t="s">
-        <v>236</v>
-      </c>
-      <c r="C35" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>279</v>
-      </c>
-      <c r="B36" t="s">
-        <v>237</v>
-      </c>
-      <c r="C36" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" t="s">
-        <v>238</v>
-      </c>
-      <c r="C37" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>280</v>
-      </c>
-      <c r="B38" t="s">
-        <v>239</v>
-      </c>
-      <c r="C38" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>281</v>
-      </c>
-      <c r="B39" t="s">
-        <v>241</v>
-      </c>
-      <c r="C39" t="s">
-        <v>249</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>289</v>
       </c>
-      <c r="C40" t="s">
-        <v>250</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>290</v>
       </c>
-      <c r="C41" t="s">
-        <v>250</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>291</v>
-      </c>
-      <c r="B42" t="s">
-        <v>292</v>
-      </c>
-      <c r="C42" t="s">
-        <v>247</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
+      <c r="C43" t="s">
+        <v>245</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>0.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>